<commit_message>
evaluating phase 1st results 2
</commit_message>
<xml_diff>
--- a/knapsack_cpp/data/Presenting_Results_Final_Version.xlsx
+++ b/knapsack_cpp/data/Presenting_Results_Final_Version.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>Run your algorithm for each benchmark (e.g. SENTO1) 30 times</t>
   </si>
@@ -98,43 +98,46 @@
     <t xml:space="preserve"> problem PB6.DAT</t>
   </si>
   <si>
-    <t>727.133 ± 55.8457</t>
-  </si>
-  <si>
-    <t>9121.43 ± 3563.34</t>
-  </si>
-  <si>
     <t>7674.6 ± 100.055</t>
   </si>
   <si>
     <t>10412.5 ± 4936.15</t>
   </si>
   <si>
-    <t>8684.4 ± 23.9102</t>
-  </si>
-  <si>
-    <t>9373.53 ± 169.749</t>
-  </si>
-  <si>
-    <t>16987.5 ± 5135.23</t>
-  </si>
-  <si>
-    <t>92094.8 ± 1434.9</t>
-  </si>
-  <si>
-    <t>10116.7 ± 2614.54</t>
-  </si>
-  <si>
-    <t>2090.8 ± 20.0867</t>
-  </si>
-  <si>
-    <t>9225 ± 7601.4</t>
-  </si>
-  <si>
-    <t>732.1 ± 50.2726</t>
-  </si>
-  <si>
-    <t>7550 ± 4050.62</t>
+    <t>8681.53 ± 24.4254</t>
+  </si>
+  <si>
+    <t>16000 ± nan</t>
+  </si>
+  <si>
+    <t>92368.5 ± 1734.06</t>
+  </si>
+  <si>
+    <t>5825 ± 4504.3</t>
+  </si>
+  <si>
+    <t>728.3 ± 53.8633</t>
+  </si>
+  <si>
+    <t>7425 ± 3602.33</t>
+  </si>
+  <si>
+    <t>6476.07 ± 271.445</t>
+  </si>
+  <si>
+    <t>13125 ± 5616.88</t>
+  </si>
+  <si>
+    <t>9410.37 ± 96.6692</t>
+  </si>
+  <si>
+    <t>16137.5 ± 6844.75</t>
+  </si>
+  <si>
+    <t>2084.93 ± 26.2651</t>
+  </si>
+  <si>
+    <t>17700 ± 70.7107</t>
   </si>
 </sst>
 </file>
@@ -620,7 +623,7 @@
   <dimension ref="A1:I60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -631,7 +634,7 @@
     <col min="4" max="4" width="20.33203125" customWidth="1"/>
     <col min="5" max="5" width="19" customWidth="1"/>
     <col min="6" max="6" width="19.6640625" customWidth="1"/>
-    <col min="7" max="7" width="14.5" customWidth="1"/>
+    <col min="7" max="7" width="17.33203125" customWidth="1"/>
     <col min="8" max="8" width="19.83203125" customWidth="1"/>
     <col min="9" max="9" width="20.33203125" customWidth="1"/>
     <col min="24" max="24" width="19.1640625" customWidth="1"/>
@@ -712,25 +715,25 @@
       </c>
       <c r="B10" s="8"/>
       <c r="C10" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="D10" s="18" t="s">
+      <c r="E10" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="G10" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="E10" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="F10" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="G10" s="8" t="s">
-        <v>29</v>
-      </c>
       <c r="H10" s="8" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="I10" s="7" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.15">
@@ -742,10 +745,10 @@
         <v>7772</v>
       </c>
       <c r="D11" s="8">
-        <v>8720</v>
+        <v>8722</v>
       </c>
       <c r="E11" s="8">
-        <v>776</v>
+        <v>6339</v>
       </c>
       <c r="F11" s="8">
         <v>9450</v>
@@ -769,22 +772,22 @@
         <v>7400</v>
       </c>
       <c r="D12" s="8">
-        <v>8635</v>
+        <v>8632</v>
       </c>
       <c r="E12" s="8">
-        <v>609</v>
+        <v>6912</v>
       </c>
       <c r="F12" s="8">
-        <v>8738</v>
+        <v>9177</v>
       </c>
       <c r="G12" s="8">
-        <v>90417</v>
+        <v>90444</v>
       </c>
       <c r="H12" s="8">
-        <v>2068</v>
+        <v>2025</v>
       </c>
       <c r="I12" s="7">
-        <v>601</v>
+        <v>603</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.15">
@@ -796,22 +799,22 @@
         <v>0.13333300000000001</v>
       </c>
       <c r="D13" s="18">
-        <v>0</v>
+        <v>3.3333300000000003E-2</v>
       </c>
       <c r="E13" s="9">
-        <v>0.23333300000000001</v>
+        <v>0.26666699999999999</v>
       </c>
       <c r="F13" s="18">
         <v>0.13333300000000001</v>
       </c>
       <c r="G13" s="9">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="H13" s="18">
         <v>6.6666699999999995E-2</v>
       </c>
       <c r="I13" s="20">
-        <v>0.23333300000000001</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.15">
@@ -820,23 +823,25 @@
       </c>
       <c r="B14" s="8"/>
       <c r="C14" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="D14" s="8"/>
       <c r="E14" s="8" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="H14" s="8" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="I14" s="7" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.15">
@@ -847,21 +852,23 @@
       <c r="C15" s="8">
         <v>7050</v>
       </c>
-      <c r="D15" s="8"/>
+      <c r="D15" s="8">
+        <v>16000</v>
+      </c>
       <c r="E15" s="8">
-        <v>4900</v>
+        <v>7800</v>
       </c>
       <c r="F15" s="8">
-        <v>11300</v>
+        <v>8750</v>
       </c>
       <c r="G15" s="8">
-        <v>7200</v>
+        <v>3150</v>
       </c>
       <c r="H15" s="8">
-        <v>3850</v>
+        <v>17650</v>
       </c>
       <c r="I15" s="7">
-        <v>3950</v>
+        <v>4250</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="14" thickBot="1" x14ac:dyDescent="0.2">
@@ -872,21 +879,23 @@
       <c r="C16" s="10">
         <v>17700</v>
       </c>
-      <c r="D16" s="10"/>
+      <c r="D16" s="10">
+        <v>16000</v>
+      </c>
       <c r="E16" s="10">
-        <v>13000</v>
+        <v>21750</v>
       </c>
       <c r="F16" s="10">
-        <v>21650</v>
+        <v>23950</v>
       </c>
       <c r="G16" s="10">
-        <v>12250</v>
+        <v>14900</v>
       </c>
       <c r="H16" s="10">
-        <v>14600</v>
+        <v>17750</v>
       </c>
       <c r="I16" s="11">
-        <v>15600</v>
+        <v>14150</v>
       </c>
     </row>
     <row r="59" spans="2:2" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
evaluating phase 1st results 3
</commit_message>
<xml_diff>
--- a/knapsack_cpp/data/Presenting_Results_Final_Version.xlsx
+++ b/knapsack_cpp/data/Presenting_Results_Final_Version.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>Run your algorithm for each benchmark (e.g. SENTO1) 30 times</t>
   </si>
@@ -74,9 +74,6 @@
     <t>Compare with other algorithms</t>
   </si>
   <si>
-    <t>example Problem</t>
-  </si>
-  <si>
     <t xml:space="preserve"> problem SENTO1.DAT</t>
   </si>
   <si>
@@ -98,18 +95,6 @@
     <t xml:space="preserve"> problem PB6.DAT</t>
   </si>
   <si>
-    <t>7674.6 ± 100.055</t>
-  </si>
-  <si>
-    <t>10412.5 ± 4936.15</t>
-  </si>
-  <si>
-    <t>8681.53 ± 24.4254</t>
-  </si>
-  <si>
-    <t>16000 ± nan</t>
-  </si>
-  <si>
     <t>92368.5 ± 1734.06</t>
   </si>
   <si>
@@ -138,13 +123,25 @@
   </si>
   <si>
     <t>17700 ± 70.7107</t>
+  </si>
+  <si>
+    <t>7707.83 ± 69.0717</t>
+  </si>
+  <si>
+    <t>14062.5 ± 4563.81</t>
+  </si>
+  <si>
+    <t>8685.1 ± 22.2747</t>
+  </si>
+  <si>
+    <t>11125 ± 2863.78</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -153,6 +150,12 @@
     <font>
       <b/>
       <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -321,7 +324,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -335,14 +338,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -620,10 +626,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I60"/>
+  <dimension ref="A1:H60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -648,30 +654,30 @@
     <col min="48" max="48" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="14" thickBot="1" x14ac:dyDescent="0.2"/>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:8" ht="14" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A8" s="8"/>
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="15" t="s">
         <v>4</v>
       </c>
       <c r="C8" s="5"/>
@@ -679,222 +685,211 @@
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="6"/>
-    </row>
-    <row r="9" spans="1:9" ht="14" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="H8" s="6"/>
+    </row>
+    <row r="9" spans="1:8" ht="14" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A9" s="8"/>
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="12" t="s">
         <v>15</v>
       </c>
       <c r="D9" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="12" t="s">
+      <c r="E9" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="F9" s="15" t="s">
+      <c r="F9" s="13" t="s">
         <v>18</v>
       </c>
       <c r="G9" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="H9" s="15" t="s">
+      <c r="H9" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="I9" s="19" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10" s="18" t="s">
-        <v>24</v>
+      <c r="B10" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>25</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="F10" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="G10" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="H10" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="I10" s="7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
+        <v>27</v>
+      </c>
+      <c r="F10" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="G10" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A11" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="8"/>
+      <c r="B11" s="8">
+        <v>7772</v>
+      </c>
       <c r="C11" s="8">
-        <v>7772</v>
+        <v>8722</v>
       </c>
       <c r="D11" s="8">
-        <v>8722</v>
+        <v>6339</v>
       </c>
       <c r="E11" s="8">
-        <v>6339</v>
-      </c>
-      <c r="F11" s="8">
         <v>9450</v>
       </c>
-      <c r="G11" s="8">
+      <c r="F11" s="20">
         <v>95168</v>
       </c>
-      <c r="H11" s="8">
+      <c r="G11" s="20">
         <v>2139</v>
       </c>
-      <c r="I11" s="7">
+      <c r="H11" s="7">
         <v>776</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A12" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="8"/>
+      <c r="B12" s="8">
+        <v>7520</v>
+      </c>
       <c r="C12" s="8">
-        <v>7400</v>
+        <v>8629</v>
       </c>
       <c r="D12" s="8">
-        <v>8632</v>
+        <v>6912</v>
       </c>
       <c r="E12" s="8">
-        <v>6912</v>
-      </c>
-      <c r="F12" s="8">
         <v>9177</v>
       </c>
-      <c r="G12" s="8">
+      <c r="F12" s="20">
         <v>90444</v>
       </c>
-      <c r="H12" s="8">
+      <c r="G12" s="20">
         <v>2025</v>
       </c>
-      <c r="I12" s="7">
+      <c r="H12" s="7">
         <v>603</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A13" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="8"/>
-      <c r="C13" s="9">
+      <c r="B13" s="9">
+        <v>0.26666699999999999</v>
+      </c>
+      <c r="C13" s="16">
+        <v>6.6666699999999995E-2</v>
+      </c>
+      <c r="D13" s="9">
+        <v>0.26666699999999999</v>
+      </c>
+      <c r="E13" s="16">
         <v>0.13333300000000001</v>
       </c>
-      <c r="D13" s="18">
-        <v>3.3333300000000003E-2</v>
-      </c>
-      <c r="E13" s="9">
-        <v>0.26666699999999999</v>
-      </c>
-      <c r="F13" s="18">
-        <v>0.13333300000000001</v>
-      </c>
-      <c r="G13" s="9">
+      <c r="F13" s="21">
         <v>0.2</v>
       </c>
+      <c r="G13" s="22">
+        <v>6.6666699999999995E-2</v>
+      </c>
       <c r="H13" s="18">
-        <v>6.6666699999999995E-2</v>
-      </c>
-      <c r="I13" s="20">
         <v>0.2</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A14" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="8"/>
+      <c r="B14" s="8" t="s">
+        <v>32</v>
+      </c>
       <c r="C14" s="8" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="F14" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="G14" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="H14" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="I14" s="7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.15">
+        <v>28</v>
+      </c>
+      <c r="F14" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="G14" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="H14" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A15" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="8"/>
+      <c r="B15" s="8">
+        <v>8400</v>
+      </c>
       <c r="C15" s="8">
-        <v>7050</v>
+        <v>9100</v>
       </c>
       <c r="D15" s="8">
-        <v>16000</v>
+        <v>7800</v>
       </c>
       <c r="E15" s="8">
-        <v>7800</v>
-      </c>
-      <c r="F15" s="8">
         <v>8750</v>
       </c>
-      <c r="G15" s="8">
+      <c r="F15" s="20">
         <v>3150</v>
       </c>
-      <c r="H15" s="8">
+      <c r="G15" s="20">
         <v>17650</v>
       </c>
-      <c r="I15" s="7">
+      <c r="H15" s="7">
         <v>4250</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="14" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" ht="14" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B16" s="10"/>
+      <c r="B16" s="10">
+        <v>20250</v>
+      </c>
       <c r="C16" s="10">
-        <v>17700</v>
+        <v>13150</v>
       </c>
       <c r="D16" s="10">
-        <v>16000</v>
+        <v>21750</v>
       </c>
       <c r="E16" s="10">
-        <v>21750</v>
-      </c>
-      <c r="F16" s="10">
         <v>23950</v>
       </c>
-      <c r="G16" s="10">
+      <c r="F16" s="23">
         <v>14900</v>
       </c>
-      <c r="H16" s="10">
+      <c r="G16" s="23">
         <v>17750</v>
       </c>
-      <c r="I16" s="11">
+      <c r="H16" s="11">
         <v>14150</v>
       </c>
     </row>

</xml_diff>

<commit_message>
evaluating phase + comparison table
</commit_message>
<xml_diff>
--- a/knapsack_cpp/data/Presenting_Results_Final_Version.xlsx
+++ b/knapsack_cpp/data/Presenting_Results_Final_Version.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2500" yWindow="1480" windowWidth="20640" windowHeight="11760" tabRatio="989"/>
+    <workbookView xWindow="13460" yWindow="7800" windowWidth="15400" windowHeight="11760" tabRatio="989"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="48">
   <si>
     <t>Run your algorithm for each benchmark (e.g. SENTO1) 30 times</t>
   </si>
@@ -107,12 +107,6 @@
     <t>7425 ± 3602.33</t>
   </si>
   <si>
-    <t>6476.07 ± 271.445</t>
-  </si>
-  <si>
-    <t>13125 ± 5616.88</t>
-  </si>
-  <si>
     <t>9410.37 ± 96.6692</t>
   </si>
   <si>
@@ -135,13 +129,58 @@
   </si>
   <si>
     <t>15316.7 ± 5605.41</t>
+  </si>
+  <si>
+    <t>6655.9 ± 419.913</t>
+  </si>
+  <si>
+    <t>12270.8 ± 5909.41</t>
+  </si>
+  <si>
+    <t>PBPSO</t>
+  </si>
+  <si>
+    <t>DBDFO</t>
+  </si>
+  <si>
+    <t>Algorithm Executed 20 time</t>
+  </si>
+  <si>
+    <t>They evaluate in "iterations"</t>
+  </si>
+  <si>
+    <t>Notes:</t>
+  </si>
+  <si>
+    <t>KBPSO</t>
+  </si>
+  <si>
+    <t>MBPSO</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>BEST KNOWN:</t>
+  </si>
+  <si>
+    <t>Avg Efficiency</t>
+  </si>
+  <si>
+    <t>Average Fitness</t>
+  </si>
+  <si>
+    <t>DE</t>
+  </si>
+  <si>
+    <t>SD-BDE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -156,6 +195,12 @@
     <font>
       <sz val="10"/>
       <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -180,12 +225,27 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="19">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -275,17 +335,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="0"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color auto="1"/>
       </left>
@@ -308,14 +357,84 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right style="medium">
         <color auto="1"/>
       </right>
       <top style="thin">
-        <color theme="0"/>
+        <color auto="1"/>
       </top>
-      <bottom style="medium">
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
         <color auto="1"/>
       </bottom>
       <diagonal/>
@@ -324,33 +443,45 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -628,10 +759,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H60"/>
+  <dimension ref="A1:I54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -656,257 +787,1066 @@
     <col min="48" max="48" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B1" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="C1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B2" t="s">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="C2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B3" t="s">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="C3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B4" t="s">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="C4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="14" thickBot="1" x14ac:dyDescent="0.2"/>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A8" s="9"/>
-      <c r="B8" s="16" t="s">
+    <row r="6" spans="1:9" ht="14" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="C7" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="7"/>
-    </row>
-    <row r="9" spans="1:8" ht="14" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="9"/>
-      <c r="B9" s="20" t="s">
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="6"/>
+    </row>
+    <row r="8" spans="1:9" ht="14" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="C8" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="D8" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="13" t="s">
+      <c r="E8" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="15" t="s">
+      <c r="F8" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="F9" s="14" t="s">
+      <c r="G8" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="G9" s="15" t="s">
+      <c r="H8" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="H9" s="18" t="s">
+      <c r="I8" s="32" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A10" s="3" t="s">
+    <row r="9" spans="1:9" ht="14" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="36" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" s="22">
+        <v>7772</v>
+      </c>
+      <c r="D9" s="10">
+        <v>8722</v>
+      </c>
+      <c r="E9" s="10">
+        <v>6339</v>
+      </c>
+      <c r="F9" s="27">
+        <v>9450</v>
+      </c>
+      <c r="G9" s="27">
+        <v>95168</v>
+      </c>
+      <c r="H9" s="27">
+        <v>2139</v>
+      </c>
+      <c r="I9" s="28">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A10" s="25" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="C10" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C10" s="17" t="s">
+      <c r="F10" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="G10" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="H10" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="D10" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="E10" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="F10" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="G10" s="24" t="s">
-        <v>31</v>
-      </c>
-      <c r="H10" s="8" t="s">
+      <c r="I10" s="7" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A11" s="4" t="s">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="9">
+      <c r="C11" s="8">
         <v>7772</v>
       </c>
-      <c r="C11" s="9">
+      <c r="D11" s="8">
         <v>8722</v>
       </c>
-      <c r="D11" s="9">
+      <c r="E11" s="8">
         <v>6339</v>
       </c>
-      <c r="E11" s="9">
+      <c r="F11" s="8">
         <v>9450</v>
       </c>
-      <c r="F11" s="21">
+      <c r="G11" s="15">
         <v>95168</v>
       </c>
-      <c r="G11" s="24">
+      <c r="H11" s="18">
         <v>2139</v>
       </c>
-      <c r="H11" s="8">
+      <c r="I11" s="7">
         <v>776</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A12" s="4" t="s">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="9">
+      <c r="C12" s="8">
         <v>7443</v>
       </c>
-      <c r="C12" s="9">
+      <c r="D12" s="8">
         <v>8629</v>
       </c>
-      <c r="D12" s="9">
-        <v>6912</v>
-      </c>
-      <c r="E12" s="9">
+      <c r="E12" s="8">
+        <v>7201</v>
+      </c>
+      <c r="F12" s="8">
         <v>9177</v>
       </c>
-      <c r="F12" s="21">
+      <c r="G12" s="15">
         <v>90444</v>
       </c>
-      <c r="G12" s="24">
+      <c r="H12" s="18">
         <v>2059</v>
       </c>
-      <c r="H12" s="8">
+      <c r="I12" s="7">
         <v>603</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A13" s="4" t="s">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="10">
+      <c r="C13" s="9">
         <v>0.2</v>
       </c>
-      <c r="C13" s="17">
+      <c r="D13" s="13">
         <v>6.6666699999999995E-2</v>
       </c>
-      <c r="D13" s="10">
-        <v>0.26666699999999999</v>
-      </c>
-      <c r="E13" s="17">
+      <c r="E13" s="9">
+        <v>0.4</v>
+      </c>
+      <c r="F13" s="13">
         <v>0.13333300000000001</v>
       </c>
-      <c r="F13" s="22">
+      <c r="G13" s="16">
         <v>0.2</v>
       </c>
-      <c r="G13" s="25">
+      <c r="H13" s="19">
         <v>0.1</v>
       </c>
-      <c r="H13" s="19">
+      <c r="I13" s="14">
         <v>0.2</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A14" s="4" t="s">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="C14" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E14" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="C14" s="9" t="s">
+      <c r="F14" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G14" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="H14" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="D14" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="E14" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="F14" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="G14" s="24" t="s">
-        <v>32</v>
-      </c>
-      <c r="H14" s="8" t="s">
+      <c r="I14" s="7" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A15" s="4" t="s">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="9">
+      <c r="C15" s="8">
         <v>9100</v>
       </c>
-      <c r="C15" s="9">
+      <c r="D15" s="8">
         <v>9100</v>
       </c>
-      <c r="D15" s="9">
-        <v>7800</v>
-      </c>
-      <c r="E15" s="9">
+      <c r="E15" s="8">
+        <v>5850</v>
+      </c>
+      <c r="F15" s="8">
         <v>8750</v>
       </c>
-      <c r="F15" s="21">
+      <c r="G15" s="15">
         <v>3150</v>
       </c>
-      <c r="G15" s="24">
+      <c r="H15" s="18">
         <v>950</v>
       </c>
-      <c r="H15" s="8">
+      <c r="I15" s="7">
         <v>4250</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="14" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="5" t="s">
+    <row r="16" spans="1:9" ht="14" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="4"/>
+      <c r="B16" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B16" s="11">
+      <c r="C16" s="10">
         <v>22000</v>
       </c>
-      <c r="C16" s="11">
+      <c r="D16" s="10">
         <v>13150</v>
       </c>
-      <c r="D16" s="11">
-        <v>21750</v>
-      </c>
-      <c r="E16" s="11">
+      <c r="E16" s="10">
+        <v>20000</v>
+      </c>
+      <c r="F16" s="10">
         <v>23950</v>
       </c>
-      <c r="F16" s="23">
+      <c r="G16" s="17">
         <v>14900</v>
       </c>
-      <c r="G16" s="23">
+      <c r="H16" s="17">
         <v>9700</v>
       </c>
-      <c r="H16" s="12">
+      <c r="I16" s="11">
         <v>14150</v>
       </c>
     </row>
-    <row r="26" spans="6:6" x14ac:dyDescent="0.15">
-      <c r="F26" s="2"/>
-    </row>
-    <row r="59" spans="2:2" x14ac:dyDescent="0.15">
-      <c r="B59" s="1" t="s">
+    <row r="17" spans="1:9" ht="14" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="C18" s="33" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="60" spans="2:2" x14ac:dyDescent="0.15">
-      <c r="B60" t="s">
+      <c r="D18" s="34"/>
+      <c r="E18" s="34"/>
+      <c r="F18" s="34"/>
+      <c r="G18" s="34"/>
+      <c r="H18" s="34"/>
+      <c r="I18" s="35"/>
+    </row>
+    <row r="19" spans="1:9" ht="14" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="C19" s="22" t="s">
         <v>13</v>
       </c>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="10"/>
+      <c r="H19" s="10"/>
+      <c r="I19" s="11"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A20" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C20" s="20">
+        <v>7695.9</v>
+      </c>
+      <c r="D20" s="5">
+        <v>8671.1</v>
+      </c>
+      <c r="E20" s="5">
+        <v>6331.75</v>
+      </c>
+      <c r="F20" s="5">
+        <v>9362.0499999999993</v>
+      </c>
+      <c r="G20" s="5">
+        <v>93114.1</v>
+      </c>
+      <c r="H20" s="5">
+        <v>2134.4499999999998</v>
+      </c>
+      <c r="I20" s="6">
+        <v>752.85</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A21" s="3"/>
+      <c r="B21" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" s="21">
+        <v>7772</v>
+      </c>
+      <c r="D21" s="8">
+        <v>8722</v>
+      </c>
+      <c r="E21" s="8">
+        <v>6339</v>
+      </c>
+      <c r="F21" s="24">
+        <v>9450</v>
+      </c>
+      <c r="G21" s="8">
+        <v>95168</v>
+      </c>
+      <c r="H21" s="8">
+        <v>2139</v>
+      </c>
+      <c r="I21" s="7">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A22" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" s="23"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="7"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A23" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23" s="23">
+        <v>0.05</v>
+      </c>
+      <c r="D23" s="9">
+        <v>0.05</v>
+      </c>
+      <c r="E23" s="9">
+        <v>0.45</v>
+      </c>
+      <c r="F23" s="9">
+        <v>0.05</v>
+      </c>
+      <c r="G23" s="9">
+        <v>0.4</v>
+      </c>
+      <c r="H23" s="9">
+        <v>0.75</v>
+      </c>
+      <c r="I23" s="14">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A24" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C24" s="21">
+        <v>3158</v>
+      </c>
+      <c r="D24" s="24">
+        <v>2221</v>
+      </c>
+      <c r="E24" s="24">
+        <v>1436</v>
+      </c>
+      <c r="F24" s="24">
+        <v>3652</v>
+      </c>
+      <c r="G24" s="8">
+        <v>729</v>
+      </c>
+      <c r="H24" s="8">
+        <v>1012</v>
+      </c>
+      <c r="I24" s="7">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A25" s="3"/>
+      <c r="B25" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C25" s="21">
+        <v>3158</v>
+      </c>
+      <c r="D25" s="24">
+        <v>2221</v>
+      </c>
+      <c r="E25" s="24">
+        <v>112</v>
+      </c>
+      <c r="F25" s="8"/>
+      <c r="G25" s="8">
+        <v>181</v>
+      </c>
+      <c r="H25" s="8">
+        <v>129</v>
+      </c>
+      <c r="I25" s="7">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="14" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="4"/>
+      <c r="B26" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C26" s="22"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="10"/>
+      <c r="F26" s="10"/>
+      <c r="G26" s="10"/>
+      <c r="H26" s="10"/>
+      <c r="I26" s="11"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A27" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C27" s="5">
+        <v>7562.4</v>
+      </c>
+      <c r="D27" s="5">
+        <v>8671.1</v>
+      </c>
+      <c r="E27" s="5">
+        <v>6331.75</v>
+      </c>
+      <c r="F27" s="5">
+        <v>9362.0499999999993</v>
+      </c>
+      <c r="G27" s="5">
+        <v>93114.1</v>
+      </c>
+      <c r="H27" s="5">
+        <v>2134.4499999999998</v>
+      </c>
+      <c r="I27" s="6">
+        <v>752.85</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A28" s="3"/>
+      <c r="B28" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C28" s="8">
+        <v>7676</v>
+      </c>
+      <c r="D28" s="8">
+        <v>8722</v>
+      </c>
+      <c r="E28" s="8">
+        <v>6339</v>
+      </c>
+      <c r="F28" s="24">
+        <v>9450</v>
+      </c>
+      <c r="G28" s="8">
+        <v>95168</v>
+      </c>
+      <c r="H28" s="8">
+        <v>2139</v>
+      </c>
+      <c r="I28" s="7">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A29" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C29" s="9"/>
+      <c r="G29" s="8"/>
+      <c r="H29" s="8"/>
+      <c r="I29" s="7"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A30" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C30" s="9">
+        <v>0</v>
+      </c>
+      <c r="D30" s="9">
+        <v>0</v>
+      </c>
+      <c r="E30" s="9">
+        <v>0.15</v>
+      </c>
+      <c r="F30" s="9">
+        <v>0</v>
+      </c>
+      <c r="G30" s="9">
+        <v>0.2</v>
+      </c>
+      <c r="H30" s="9">
+        <v>0.65</v>
+      </c>
+      <c r="I30" s="14">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A31" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D31" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="E31" s="24">
+        <v>2600</v>
+      </c>
+      <c r="F31" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="G31" s="8">
+        <v>1304</v>
+      </c>
+      <c r="H31" s="8">
+        <v>1078</v>
+      </c>
+      <c r="I31" s="7">
+        <v>2640</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A32" s="3"/>
+      <c r="B32" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D32" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="E32" s="24">
+        <v>2183</v>
+      </c>
+      <c r="F32" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="G32" s="8">
+        <v>438</v>
+      </c>
+      <c r="H32" s="8">
+        <v>97</v>
+      </c>
+      <c r="I32" s="7">
+        <v>2495</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="14" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="4"/>
+      <c r="B33" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C33" s="10"/>
+      <c r="D33" s="10"/>
+      <c r="E33" s="10"/>
+      <c r="F33" s="10"/>
+      <c r="G33" s="10"/>
+      <c r="H33" s="10"/>
+      <c r="I33" s="11"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A34" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C34" s="20">
+        <v>7683.55</v>
+      </c>
+      <c r="D34" s="5">
+        <v>8651</v>
+      </c>
+      <c r="E34" s="5">
+        <v>6317.05</v>
+      </c>
+      <c r="F34" s="5">
+        <v>9352.9500000000007</v>
+      </c>
+      <c r="G34" s="5">
+        <v>92419</v>
+      </c>
+      <c r="H34" s="5">
+        <v>2110.9</v>
+      </c>
+      <c r="I34" s="6">
+        <v>708.6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A35" s="3"/>
+      <c r="B35" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C35" s="21">
+        <v>7762</v>
+      </c>
+      <c r="D35" s="8">
+        <v>8711</v>
+      </c>
+      <c r="E35" s="24">
+        <v>6339</v>
+      </c>
+      <c r="F35" s="24">
+        <v>9445</v>
+      </c>
+      <c r="G35" s="24">
+        <v>95168</v>
+      </c>
+      <c r="H35" s="24">
+        <v>2139</v>
+      </c>
+      <c r="I35" s="7">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A36" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C36" s="23"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+      <c r="G36" s="9"/>
+      <c r="H36" s="9"/>
+      <c r="I36" s="14"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A37" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C37" s="23">
+        <v>0</v>
+      </c>
+      <c r="D37" s="1">
+        <v>0</v>
+      </c>
+      <c r="E37" s="1">
+        <v>0.35</v>
+      </c>
+      <c r="F37" s="1">
+        <v>0</v>
+      </c>
+      <c r="G37" s="9">
+        <v>0.15</v>
+      </c>
+      <c r="H37" s="9">
+        <v>0.05</v>
+      </c>
+      <c r="I37" s="14">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A38" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C38" s="21"/>
+      <c r="D38" s="24"/>
+      <c r="E38" s="24">
+        <v>2162</v>
+      </c>
+      <c r="F38" s="24"/>
+      <c r="G38" s="24">
+        <v>1744</v>
+      </c>
+      <c r="H38" s="8">
+        <v>90</v>
+      </c>
+      <c r="I38" s="7">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A39" s="3"/>
+      <c r="B39" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C39" s="21"/>
+      <c r="D39" s="24"/>
+      <c r="E39" s="24">
+        <v>890</v>
+      </c>
+      <c r="F39" s="8"/>
+      <c r="G39" s="24">
+        <v>540</v>
+      </c>
+      <c r="H39" s="8">
+        <v>90</v>
+      </c>
+      <c r="I39" s="7">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="14" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="4"/>
+      <c r="B40" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C40" s="22"/>
+      <c r="D40" s="10"/>
+      <c r="E40" s="10"/>
+      <c r="F40" s="10"/>
+      <c r="G40" s="10"/>
+      <c r="H40" s="10"/>
+      <c r="I40" s="11"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A41" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C41" s="5">
+        <v>7765.25</v>
+      </c>
+      <c r="D41" s="5">
+        <v>8709.9500000000007</v>
+      </c>
+      <c r="E41" s="5">
+        <v>6329.35</v>
+      </c>
+      <c r="F41" s="5">
+        <v>9450</v>
+      </c>
+      <c r="G41" s="5">
+        <v>95089.65</v>
+      </c>
+      <c r="H41" s="5">
+        <v>2119.5500000000002</v>
+      </c>
+      <c r="I41" s="6">
+        <v>734.6</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A42" s="3"/>
+      <c r="B42" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C42" s="8">
+        <v>7772</v>
+      </c>
+      <c r="D42" s="8">
+        <v>8721</v>
+      </c>
+      <c r="E42" s="24">
+        <v>6339</v>
+      </c>
+      <c r="F42" s="24">
+        <v>9442.75</v>
+      </c>
+      <c r="G42" s="24">
+        <v>95168</v>
+      </c>
+      <c r="H42" s="24">
+        <v>2139</v>
+      </c>
+      <c r="I42" s="7">
+        <v>765</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A43" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C43" s="9"/>
+      <c r="G43" s="8"/>
+      <c r="H43" s="8"/>
+      <c r="I43" s="7"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A44" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C44" s="9">
+        <v>0.1</v>
+      </c>
+      <c r="D44" s="9">
+        <v>0</v>
+      </c>
+      <c r="E44" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="F44" s="9">
+        <v>0.7</v>
+      </c>
+      <c r="G44" s="9">
+        <v>0.9</v>
+      </c>
+      <c r="H44" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="I44" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A45" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C45" s="8"/>
+      <c r="D45" s="24"/>
+      <c r="E45" s="24"/>
+      <c r="F45" s="24"/>
+      <c r="G45" s="8"/>
+      <c r="H45" s="8"/>
+      <c r="I45" s="7"/>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A46" s="3"/>
+      <c r="B46" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C46" s="8"/>
+      <c r="D46" s="24"/>
+      <c r="E46" s="24"/>
+      <c r="F46" s="24"/>
+      <c r="G46" s="8"/>
+      <c r="H46" s="8"/>
+      <c r="I46" s="7"/>
+    </row>
+    <row r="47" spans="1:9" ht="14" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="4"/>
+      <c r="B47" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C47" s="8"/>
+      <c r="D47" s="8"/>
+      <c r="E47" s="8"/>
+      <c r="F47" s="8"/>
+      <c r="G47" s="8"/>
+      <c r="H47" s="8"/>
+      <c r="I47" s="7"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A48" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C48" s="20">
+        <v>7765.25</v>
+      </c>
+      <c r="D48" s="5">
+        <v>8721.0499999999993</v>
+      </c>
+      <c r="E48" s="37">
+        <v>6339</v>
+      </c>
+      <c r="F48" s="5">
+        <v>9450</v>
+      </c>
+      <c r="G48" s="5">
+        <v>95147.7</v>
+      </c>
+      <c r="H48" s="5">
+        <v>2130.35</v>
+      </c>
+      <c r="I48" s="6">
+        <v>764.55</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A49" s="3"/>
+      <c r="B49" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C49" s="21">
+        <v>7772</v>
+      </c>
+      <c r="D49" s="8">
+        <v>8721</v>
+      </c>
+      <c r="E49" s="24">
+        <v>6339</v>
+      </c>
+      <c r="F49" s="8">
+        <v>9450</v>
+      </c>
+      <c r="G49" s="24">
+        <v>95168</v>
+      </c>
+      <c r="H49" s="24">
+        <v>2139</v>
+      </c>
+      <c r="I49" s="7">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A50" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C50" s="23"/>
+      <c r="D50" s="8"/>
+      <c r="E50" s="8"/>
+      <c r="F50" s="8"/>
+      <c r="G50" s="8"/>
+      <c r="H50" s="8"/>
+      <c r="I50" s="7"/>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A51" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C51" s="23">
+        <v>0.4</v>
+      </c>
+      <c r="D51" s="9">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="E51" s="9">
+        <v>1</v>
+      </c>
+      <c r="F51" s="9">
+        <v>1</v>
+      </c>
+      <c r="G51" s="9">
+        <v>0.9</v>
+      </c>
+      <c r="H51" s="9">
+        <v>0.6</v>
+      </c>
+      <c r="I51" s="14">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A52" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C52" s="21"/>
+      <c r="D52" s="24"/>
+      <c r="E52" s="24"/>
+      <c r="F52" s="24"/>
+      <c r="G52" s="8"/>
+      <c r="H52" s="8"/>
+      <c r="I52" s="7"/>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A53" s="3"/>
+      <c r="B53" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C53" s="21"/>
+      <c r="D53" s="24"/>
+      <c r="E53" s="24"/>
+      <c r="F53" s="24"/>
+      <c r="G53" s="8"/>
+      <c r="H53" s="8"/>
+      <c r="I53" s="7"/>
+    </row>
+    <row r="54" spans="1:9" ht="14" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="4"/>
+      <c r="B54" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C54" s="22"/>
+      <c r="D54" s="10"/>
+      <c r="E54" s="10"/>
+      <c r="F54" s="10"/>
+      <c r="G54" s="10"/>
+      <c r="H54" s="10"/>
+      <c r="I54" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>

</xml_diff>